<commit_message>
Plan de Formacion Individual Actualizado v0.8
</commit_message>
<xml_diff>
--- a/media/excels/cuadros.xlsx
+++ b/media/excels/cuadros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos en Ejecucion\Cantera Joven Cujae\Cantera Joven CUJAE Backend\media\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF70C457-1284-4C2B-BD0E-C4E15A044BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DF30C5-0FF7-4E9B-BF97-6586CBB84328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>Nombre</t>
   </si>
@@ -492,7 +492,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,6 +615,9 @@
       <c r="D6">
         <v>89031256474</v>
       </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -629,6 +632,9 @@
       <c r="D7">
         <v>80091878977</v>
       </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -643,6 +649,9 @@
       <c r="D8">
         <v>79081872209</v>
       </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -707,6 +716,9 @@
       </c>
       <c r="D12">
         <v>78091878909</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>